<commit_message>
Modificando los reportes sgc solicitados por el auditor
</commit_message>
<xml_diff>
--- a/styles/documentos/sgc_resumen.xlsx
+++ b/styles/documentos/sgc_resumen.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\sitioProduccion02\styles\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp54\htdocs\xevanes\styles\documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>Nº</t>
   </si>
@@ -56,15 +56,9 @@
     <t>Certificados de Origen Repuestos</t>
   </si>
   <si>
-    <t>Número de depósitos presentados</t>
-  </si>
-  <si>
     <t>No. Total de Certificados de Origen Repuestos</t>
   </si>
   <si>
-    <t>Depósitos Rechazados por la UAF</t>
-  </si>
-  <si>
     <t>Solicitudes de Registro atendidos en el tiempo establecido (RUEX)</t>
   </si>
   <si>
@@ -86,12 +80,6 @@
     <t>No. Total de solicitudes recibidas</t>
   </si>
   <si>
-    <t>6,1</t>
-  </si>
-  <si>
-    <t>6,2</t>
-  </si>
-  <si>
     <t>7,1</t>
   </si>
   <si>
@@ -140,13 +128,7 @@
     <t>15,2</t>
   </si>
   <si>
-    <t>UAF</t>
-  </si>
-  <si>
     <t>UCO</t>
-  </si>
-  <si>
-    <t>No. de depósitos rechazados</t>
   </si>
   <si>
     <t>No. de facturas anuladas</t>
@@ -449,6 +431,36 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,47 +473,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -810,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S25"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,14 +830,14 @@
       <c r="S1" s="3"/>
     </row>
     <row r="2" spans="1:19" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -940,20 +922,20 @@
       <c r="S5" s="3"/>
     </row>
     <row r="6" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
+      <c r="A6" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="34" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="19"/>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="42" t="s">
+      <c r="F6" s="34" t="s">
         <v>1</v>
       </c>
       <c r="G6" s="7"/>
@@ -971,12 +953,12 @@
       <c r="S6" s="7"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="44"/>
-      <c r="B7" s="43"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="20"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="43"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="35"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
@@ -992,269 +974,250 @@
       <c r="S7" s="7"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
-        <v>6</v>
-      </c>
-      <c r="B8" s="35" t="s">
+      <c r="A8" s="41">
+        <v>7</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" s="42"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" s="39">
+        <v>8</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" s="40"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+    </row>
+    <row r="12" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="41">
+        <v>10</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="H12" s="12"/>
+    </row>
+    <row r="13" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="42"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="39">
+        <v>11</v>
+      </c>
+      <c r="B14" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="26" t="s">
+      <c r="C14" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A15" s="40"/>
+      <c r="B15" s="31"/>
+      <c r="C15" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27" t="s">
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="45">
+        <v>12</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="22" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="31">
-        <v>7</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D10" s="16" t="s">
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="46"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="16" t="s">
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="39">
+        <v>13</v>
+      </c>
+      <c r="B18" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="29">
-        <v>8</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="36"/>
-      <c r="C13" s="25" t="s">
-        <v>26</v>
-      </c>
-      <c r="D13" s="26" t="s">
+      <c r="E18" s="27"/>
+      <c r="F18" s="27" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="40"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-    </row>
-    <row r="14" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="31">
-        <v>10</v>
-      </c>
-      <c r="B14" s="37" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="41">
         <v>14</v>
       </c>
-      <c r="C14" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="B20" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="33"/>
+      <c r="C21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="H14" s="12"/>
-    </row>
-    <row r="15" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="38"/>
-      <c r="C15" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
-        <v>11</v>
-      </c>
-      <c r="B16" s="35" t="s">
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="39">
         <v>15</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D16" s="26" t="s">
+      <c r="B22" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="D22" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="36"/>
-      <c r="C17" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="33">
-        <v>12</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="22" t="s">
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="40"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="34"/>
-      <c r="B19" s="40"/>
-      <c r="C19" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="29">
-        <v>13</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="C20" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="26" t="s">
-        <v>49</v>
-      </c>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D21" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="31">
-        <v>14</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="38"/>
-      <c r="C23" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="29">
-        <v>15</v>
-      </c>
-      <c r="B24" s="35" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="36"/>
-      <c r="C25" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="24">
+  <mergeCells count="22">
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="F6:F7"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -1262,19 +1225,6 @@
     <mergeCell ref="E6:E7"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>